<commit_message>
DB descriptive analysis + visualization
</commit_message>
<xml_diff>
--- a/xx_overview/20221004_Auswertung_Metriken.xlsx
+++ b/xx_overview/20221004_Auswertung_Metriken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga84kuj\Documents\R\Multilab_Analysis\xx_overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B7182A-8041-4142-AE08-46ED1A0E000B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9624222C-DE41-4305-8BCC-5804F9DC7BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="375" xr2:uid="{E862D693-EF21-44AF-8D63-EF763FEB6A34}"/>
   </bookViews>
@@ -2259,8 +2259,8 @@
   </sheetPr>
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="C34:D39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3256,7 +3256,7 @@
         <v>111</v>
       </c>
       <c r="D34" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E34" s="82" t="s">
         <v>128</v>
@@ -3290,7 +3290,7 @@
         <v>171</v>
       </c>
       <c r="D35" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E35" s="19">
         <v>0</v>
@@ -3321,7 +3321,7 @@
         <v>112</v>
       </c>
       <c r="D36" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E36" s="82" t="s">
         <v>128</v>
@@ -3352,7 +3352,7 @@
         <v>113</v>
       </c>
       <c r="D37" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E37" s="82" t="s">
         <v>128</v>
@@ -3383,7 +3383,7 @@
         <v>60</v>
       </c>
       <c r="D38" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E38" s="82" t="s">
         <v>128</v>
@@ -3417,7 +3417,7 @@
         <v>114</v>
       </c>
       <c r="D39" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E39" s="19">
         <v>0</v>

</xml_diff>